<commit_message>
rerun dist commute with harmonised education
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/accuracy_all_edit.xlsx
+++ b/outputs/ML_Results/accuracy_all_edit.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\projects\sufficcs_mobility\outputs\ML_Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{59DA0DC5-FFD2-4E60-84FB-DA9E1C0B5E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1AE83B-087E-4A13-95EB-E5B64CA7437E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accuracy_all" sheetId="1" r:id="rId1"/>
     <sheet name="accuracy_all (2)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>city</t>
   </si>
@@ -111,12 +124,18 @@
   </si>
   <si>
     <t>Düsseldorf</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -594,8 +613,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -950,11 +970,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A23" sqref="A23:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -999,7 +1019,7 @@
         <v>0.83199999999999996</v>
       </c>
       <c r="D2">
-        <v>0.18</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="E2">
         <v>0.16800000000000001</v>
@@ -1028,10 +1048,10 @@
         <v>0.19800000000000001</v>
       </c>
       <c r="D3">
-        <v>-1.4E-2</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="E3">
-        <v>-5.0000000000000001E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="F3">
         <v>0.68899999999999995</v>
@@ -1060,7 +1080,7 @@
         <v>0.108</v>
       </c>
       <c r="E4">
-        <v>3.1E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="F4">
         <v>0.65200000000000002</v>
@@ -1086,10 +1106,10 @@
         <v>-0.77800000000000002</v>
       </c>
       <c r="D5">
-        <v>-0.04</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="E5">
-        <v>1.7000000000000001E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="F5">
         <v>0.66800000000000004</v>
@@ -1115,10 +1135,10 @@
         <v>-29.032</v>
       </c>
       <c r="D6">
-        <v>-3.4000000000000002E-2</v>
+        <v>-4.3999999999999997E-2</v>
       </c>
       <c r="E6">
-        <v>-5.0000000000000001E-3</v>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="F6">
         <v>0.68500000000000005</v>
@@ -1144,10 +1164,10 @@
         <v>-1.2869999999999999</v>
       </c>
       <c r="D7">
-        <v>8.5999999999999993E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E7">
-        <v>8.3000000000000004E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="F7">
         <v>0.68400000000000005</v>
@@ -1173,10 +1193,10 @@
         <v>-2.181</v>
       </c>
       <c r="D8">
-        <v>1.6E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="E8">
-        <v>3.3000000000000002E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="F8">
         <v>0.69199999999999995</v>
@@ -1202,10 +1222,10 @@
         <v>-14.34</v>
       </c>
       <c r="D9">
-        <v>7.6999999999999999E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="E9">
-        <v>-7.0000000000000001E-3</v>
+        <v>-1.2999999999999999E-2</v>
       </c>
       <c r="F9">
         <v>0.66100000000000003</v>
@@ -1231,10 +1251,10 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="D10">
-        <v>0.22800000000000001</v>
+        <v>0.223</v>
       </c>
       <c r="E10">
-        <v>0.255</v>
+        <v>0.253</v>
       </c>
       <c r="F10">
         <v>0.91300000000000003</v>
@@ -1260,10 +1280,10 @@
         <v>0.78500000000000003</v>
       </c>
       <c r="D11">
-        <v>0.13700000000000001</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="E11">
-        <v>0.218</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="F11">
         <v>0.877</v>
@@ -1283,7 +1303,7 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="D12">
-        <v>0.115</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="E12">
         <v>0.104</v>
@@ -1306,10 +1326,10 @@
         <v>0.40699999999999997</v>
       </c>
       <c r="D13">
-        <v>0.159</v>
+        <v>0.157</v>
       </c>
       <c r="E13">
-        <v>0.152</v>
+        <v>0.151</v>
       </c>
       <c r="F13">
         <v>0.87</v>
@@ -1329,10 +1349,10 @@
         <v>0.63</v>
       </c>
       <c r="D14">
-        <v>0.217</v>
+        <v>0.216</v>
       </c>
       <c r="E14">
-        <v>0.2</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="F14">
         <v>0.875</v>
@@ -1352,10 +1372,10 @@
         <v>0.73499999999999999</v>
       </c>
       <c r="D15">
-        <v>0.192</v>
+        <v>0.193</v>
       </c>
       <c r="E15">
-        <v>0.17399999999999999</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="F15">
         <v>0.85599999999999998</v>
@@ -1378,7 +1398,7 @@
         <v>0.16800000000000001</v>
       </c>
       <c r="E16">
-        <v>0.184</v>
+        <v>0.191</v>
       </c>
       <c r="F16">
         <v>0.90900000000000003</v>
@@ -1427,10 +1447,10 @@
         <v>0.52800000000000002</v>
       </c>
       <c r="D18">
-        <v>0.18</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="E18">
-        <v>0.155</v>
+        <v>0.154</v>
       </c>
       <c r="F18">
         <v>0.86099999999999999</v>
@@ -1456,10 +1476,10 @@
         <v>0.67300000000000004</v>
       </c>
       <c r="D19">
-        <v>0.17399999999999999</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="E19">
-        <v>0.13700000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F19">
         <v>0.72799999999999998</v>
@@ -1479,10 +1499,10 @@
         <v>0.42199999999999999</v>
       </c>
       <c r="D20">
-        <v>0.11700000000000001</v>
+        <v>0.115</v>
       </c>
       <c r="E20">
-        <v>0.13700000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="F20">
         <v>0.68600000000000005</v>
@@ -1502,7 +1522,7 @@
         <v>0.45800000000000002</v>
       </c>
       <c r="D21">
-        <v>0.22</v>
+        <v>0.219</v>
       </c>
       <c r="E21">
         <v>0.182</v>
@@ -1531,7 +1551,7 @@
         <v>0.34300000000000003</v>
       </c>
       <c r="D22">
-        <v>0.113</v>
+        <v>0.11</v>
       </c>
       <c r="E22">
         <v>3.2000000000000001E-2</v>
@@ -1547,6 +1567,35 @@
       </c>
       <c r="I22">
         <v>0.79400000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="C23">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D23">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="E23">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F23">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="G23">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="H23">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="I23">
+        <v>0.76200000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1555,11 +1604,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:I20"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1605,11 +1654,11 @@
         <f>IF(accuracy_all!C2&gt;0,accuracy_all!C2,"&lt;0")</f>
         <v>0.83199999999999996</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>IF(accuracy_all!D2&gt;0,accuracy_all!D2,"&lt;0")</f>
-        <v>0.18</v>
-      </c>
-      <c r="E2">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="E2" s="1">
         <f>IF(accuracy_all!E2&gt;0,accuracy_all!E2,"&lt;0")</f>
         <v>0.16800000000000001</v>
       </c>
@@ -1642,11 +1691,11 @@
         <f>IF(accuracy_all!C3&gt;0,accuracy_all!C3,"&lt;0")</f>
         <v>0.19800000000000001</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D3" s="1" t="str">
         <f>IF(accuracy_all!D3&gt;0,accuracy_all!D3,"&lt;0")</f>
         <v>&lt;0</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E3" s="1" t="str">
         <f>IF(accuracy_all!E3&gt;0,accuracy_all!E3,"&lt;0")</f>
         <v>&lt;0</v>
       </c>
@@ -1679,13 +1728,13 @@
         <f>IF(accuracy_all!C4&gt;0,accuracy_all!C4,"&lt;0")</f>
         <v>0.46899999999999997</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f>IF(accuracy_all!D4&gt;0,accuracy_all!D4,"&lt;0")</f>
         <v>0.108</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <f>IF(accuracy_all!E4&gt;0,accuracy_all!E4,"&lt;0")</f>
-        <v>3.1E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="F4">
         <f>IF(accuracy_all!F4&gt;0,accuracy_all!F4,"&lt;0")</f>
@@ -1716,13 +1765,13 @@
         <f>IF(accuracy_all!C5&gt;0,accuracy_all!C5,"&lt;0")</f>
         <v>&lt;0</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D5" s="1" t="str">
         <f>IF(accuracy_all!D5&gt;0,accuracy_all!D5,"&lt;0")</f>
         <v>&lt;0</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <f>IF(accuracy_all!E5&gt;0,accuracy_all!E5,"&lt;0")</f>
-        <v>1.7000000000000001E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="F5">
         <f>IF(accuracy_all!F5&gt;0,accuracy_all!F5,"&lt;0")</f>
@@ -1753,11 +1802,11 @@
         <f>IF(accuracy_all!C6&gt;0,accuracy_all!C6,"&lt;0")</f>
         <v>&lt;0</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D6" s="1" t="str">
         <f>IF(accuracy_all!D6&gt;0,accuracy_all!D6,"&lt;0")</f>
         <v>&lt;0</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E6" s="1" t="str">
         <f>IF(accuracy_all!E6&gt;0,accuracy_all!E6,"&lt;0")</f>
         <v>&lt;0</v>
       </c>
@@ -1790,13 +1839,13 @@
         <f>IF(accuracy_all!C7&gt;0,accuracy_all!C7,"&lt;0")</f>
         <v>&lt;0</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <f>IF(accuracy_all!D7&gt;0,accuracy_all!D7,"&lt;0")</f>
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="E7">
+        <v>0.06</v>
+      </c>
+      <c r="E7" s="1">
         <f>IF(accuracy_all!E7&gt;0,accuracy_all!E7,"&lt;0")</f>
-        <v>8.3000000000000004E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="F7">
         <f>IF(accuracy_all!F7&gt;0,accuracy_all!F7,"&lt;0")</f>
@@ -1827,13 +1876,13 @@
         <f>IF(accuracy_all!C8&gt;0,accuracy_all!C8,"&lt;0")</f>
         <v>&lt;0</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <f>IF(accuracy_all!D8&gt;0,accuracy_all!D8,"&lt;0")</f>
-        <v>1.6E-2</v>
-      </c>
-      <c r="E8">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E8" s="1">
         <f>IF(accuracy_all!E8&gt;0,accuracy_all!E8,"&lt;0")</f>
-        <v>3.3000000000000002E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="F8">
         <f>IF(accuracy_all!F8&gt;0,accuracy_all!F8,"&lt;0")</f>
@@ -1864,11 +1913,11 @@
         <f>IF(accuracy_all!C9&gt;0,accuracy_all!C9,"&lt;0")</f>
         <v>&lt;0</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <f>IF(accuracy_all!D9&gt;0,accuracy_all!D9,"&lt;0")</f>
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="E9" t="str">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="E9" s="1" t="str">
         <f>IF(accuracy_all!E9&gt;0,accuracy_all!E9,"&lt;0")</f>
         <v>&lt;0</v>
       </c>
@@ -1901,13 +1950,13 @@
         <f>IF(accuracy_all!C10&gt;0,accuracy_all!C10,"&lt;0")</f>
         <v>0.27200000000000002</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <f>IF(accuracy_all!D10&gt;0,accuracy_all!D10,"&lt;0")</f>
-        <v>0.22800000000000001</v>
-      </c>
-      <c r="E10">
+        <v>0.223</v>
+      </c>
+      <c r="E10" s="1">
         <f>IF(accuracy_all!E10&gt;0,accuracy_all!E10,"&lt;0")</f>
-        <v>0.255</v>
+        <v>0.253</v>
       </c>
       <c r="F10">
         <f>IF(accuracy_all!F10&gt;0,accuracy_all!F10,"&lt;0")</f>
@@ -1938,13 +1987,13 @@
         <f>IF(accuracy_all!C11&gt;0,accuracy_all!C11,"&lt;0")</f>
         <v>0.78500000000000003</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <f>IF(accuracy_all!D11&gt;0,accuracy_all!D11,"&lt;0")</f>
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="E11">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="E11" s="1">
         <f>IF(accuracy_all!E11&gt;0,accuracy_all!E11,"&lt;0")</f>
-        <v>0.218</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="F11">
         <f>IF(accuracy_all!F11&gt;0,accuracy_all!F11,"&lt;0")</f>
@@ -1967,11 +2016,11 @@
         <f>IF(accuracy_all!C12&gt;0,accuracy_all!C12,"&lt;0")</f>
         <v>0.22900000000000001</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <f>IF(accuracy_all!D12&gt;0,accuracy_all!D12,"&lt;0")</f>
-        <v>0.115</v>
-      </c>
-      <c r="E12">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="E12" s="1">
         <f>IF(accuracy_all!E12&gt;0,accuracy_all!E12,"&lt;0")</f>
         <v>0.104</v>
       </c>
@@ -1996,13 +2045,13 @@
         <f>IF(accuracy_all!C13&gt;0,accuracy_all!C13,"&lt;0")</f>
         <v>0.40699999999999997</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <f>IF(accuracy_all!D13&gt;0,accuracy_all!D13,"&lt;0")</f>
-        <v>0.159</v>
-      </c>
-      <c r="E13">
+        <v>0.157</v>
+      </c>
+      <c r="E13" s="1">
         <f>IF(accuracy_all!E13&gt;0,accuracy_all!E13,"&lt;0")</f>
-        <v>0.152</v>
+        <v>0.151</v>
       </c>
       <c r="F13">
         <f>IF(accuracy_all!F13&gt;0,accuracy_all!F13,"&lt;0")</f>
@@ -2025,13 +2074,13 @@
         <f>IF(accuracy_all!C14&gt;0,accuracy_all!C14,"&lt;0")</f>
         <v>0.63</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <f>IF(accuracy_all!D14&gt;0,accuracy_all!D14,"&lt;0")</f>
-        <v>0.217</v>
-      </c>
-      <c r="E14">
+        <v>0.216</v>
+      </c>
+      <c r="E14" s="1">
         <f>IF(accuracy_all!E14&gt;0,accuracy_all!E14,"&lt;0")</f>
-        <v>0.2</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="F14">
         <f>IF(accuracy_all!F14&gt;0,accuracy_all!F14,"&lt;0")</f>
@@ -2054,13 +2103,13 @@
         <f>IF(accuracy_all!C15&gt;0,accuracy_all!C15,"&lt;0")</f>
         <v>0.73499999999999999</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <f>IF(accuracy_all!D15&gt;0,accuracy_all!D15,"&lt;0")</f>
-        <v>0.192</v>
-      </c>
-      <c r="E15">
+        <v>0.193</v>
+      </c>
+      <c r="E15" s="1">
         <f>IF(accuracy_all!E15&gt;0,accuracy_all!E15,"&lt;0")</f>
-        <v>0.17399999999999999</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="F15">
         <f>IF(accuracy_all!F15&gt;0,accuracy_all!F15,"&lt;0")</f>
@@ -2083,13 +2132,13 @@
         <f>IF(accuracy_all!C16&gt;0,accuracy_all!C16,"&lt;0")</f>
         <v>0.76300000000000001</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <f>IF(accuracy_all!D16&gt;0,accuracy_all!D16,"&lt;0")</f>
         <v>0.16800000000000001</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <f>IF(accuracy_all!E16&gt;0,accuracy_all!E16,"&lt;0")</f>
-        <v>0.184</v>
+        <v>0.191</v>
       </c>
       <c r="F16">
         <f>IF(accuracy_all!F16&gt;0,accuracy_all!F16,"&lt;0")</f>
@@ -2112,11 +2161,11 @@
         <f>IF(accuracy_all!C17&gt;0,accuracy_all!C17,"&lt;0")</f>
         <v>0.64600000000000002</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <f>IF(accuracy_all!D17&gt;0,accuracy_all!D17,"&lt;0")</f>
         <v>0.19500000000000001</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <f>IF(accuracy_all!E17&gt;0,accuracy_all!E17,"&lt;0")</f>
         <v>0.14799999999999999</v>
       </c>
@@ -2149,13 +2198,13 @@
         <f>IF(accuracy_all!C18&gt;0,accuracy_all!C18,"&lt;0")</f>
         <v>0.52800000000000002</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <f>IF(accuracy_all!D18&gt;0,accuracy_all!D18,"&lt;0")</f>
-        <v>0.18</v>
-      </c>
-      <c r="E18">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="E18" s="1">
         <f>IF(accuracy_all!E18&gt;0,accuracy_all!E18,"&lt;0")</f>
-        <v>0.155</v>
+        <v>0.154</v>
       </c>
       <c r="F18">
         <f>IF(accuracy_all!F18&gt;0,accuracy_all!F18,"&lt;0")</f>
@@ -2186,13 +2235,13 @@
         <f>IF(accuracy_all!C19&gt;0,accuracy_all!C19,"&lt;0")</f>
         <v>0.67300000000000004</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <f>IF(accuracy_all!D19&gt;0,accuracy_all!D19,"&lt;0")</f>
-        <v>0.17399999999999999</v>
-      </c>
-      <c r="E19">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="E19" s="1">
         <f>IF(accuracy_all!E19&gt;0,accuracy_all!E19,"&lt;0")</f>
-        <v>0.13700000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F19">
         <f>IF(accuracy_all!F19&gt;0,accuracy_all!F19,"&lt;0")</f>
@@ -2215,13 +2264,13 @@
         <f>IF(accuracy_all!C20&gt;0,accuracy_all!C20,"&lt;0")</f>
         <v>0.42199999999999999</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <f>IF(accuracy_all!D20&gt;0,accuracy_all!D20,"&lt;0")</f>
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="E20">
+        <v>0.115</v>
+      </c>
+      <c r="E20" s="1">
         <f>IF(accuracy_all!E20&gt;0,accuracy_all!E20,"&lt;0")</f>
-        <v>0.13700000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="F20">
         <f>IF(accuracy_all!F20&gt;0,accuracy_all!F20,"&lt;0")</f>
@@ -2244,11 +2293,11 @@
         <f>IF(accuracy_all!C21&gt;0,accuracy_all!C21,"&lt;0")</f>
         <v>0.45800000000000002</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <f>IF(accuracy_all!D21&gt;0,accuracy_all!D21,"&lt;0")</f>
-        <v>0.22</v>
-      </c>
-      <c r="E21">
+        <v>0.219</v>
+      </c>
+      <c r="E21" s="1">
         <f>IF(accuracy_all!E21&gt;0,accuracy_all!E21,"&lt;0")</f>
         <v>0.182</v>
       </c>
@@ -2281,11 +2330,11 @@
         <f>IF(accuracy_all!C22&gt;0,accuracy_all!C22,"&lt;0")</f>
         <v>0.34300000000000003</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <f>IF(accuracy_all!D22&gt;0,accuracy_all!D22,"&lt;0")</f>
-        <v>0.113</v>
-      </c>
-      <c r="E22">
+        <v>0.11</v>
+      </c>
+      <c r="E22" s="1">
         <f>IF(accuracy_all!E22&gt;0,accuracy_all!E22,"&lt;0")</f>
         <v>3.2000000000000001E-2</v>
       </c>
@@ -2304,6 +2353,37 @@
       <c r="I22">
         <f>IF(accuracy_all!I22&gt;0,accuracy_all!I22,"&lt;0")</f>
         <v>0.79400000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="C23">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D23" s="1">
+        <f>IF(accuracy_all!D23&gt;0,accuracy_all!D23,"&lt;0")</f>
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="E23" s="1">
+        <f>IF(accuracy_all!E23&gt;0,accuracy_all!E23,"&lt;0")</f>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F23">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="G23">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="H23">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="I23">
+        <v>0.76200000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun models and create results figures and tables
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/accuracy_all_edit.xlsx
+++ b/outputs/ML_Results/accuracy_all_edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\projects\sufficcs_mobility\outputs\ML_Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1AE83B-087E-4A13-95EB-E5B64CA7437E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA59A76D-790F-42E0-8C3E-AD76471488E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -974,7 +974,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:I23"/>
+      <selection activeCell="B2" sqref="B2:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1013,19 +1013,19 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>0.80800000000000005</v>
+        <v>0.80900000000000005</v>
       </c>
       <c r="C2">
         <v>0.83199999999999996</v>
       </c>
       <c r="D2">
-        <v>0.17899999999999999</v>
+        <v>0.18</v>
       </c>
       <c r="E2">
-        <v>0.16800000000000001</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="F2">
-        <v>0.67500000000000004</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="G2">
         <v>0.624</v>
@@ -1042,19 +1042,19 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>0.34</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="C3">
-        <v>0.19800000000000001</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="D3">
-        <v>-7.0000000000000001E-3</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="E3">
-        <v>-0.01</v>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="F3">
-        <v>0.68899999999999995</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="G3">
         <v>0.61599999999999999</v>
@@ -1071,22 +1071,22 @@
         <v>29</v>
       </c>
       <c r="B4">
-        <v>0.45200000000000001</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="C4">
         <v>0.46899999999999997</v>
       </c>
       <c r="D4">
-        <v>0.108</v>
+        <v>0.113</v>
       </c>
       <c r="E4">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="F4">
-        <v>0.65200000000000002</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="G4">
-        <v>0.6</v>
+        <v>0.60099999999999998</v>
       </c>
       <c r="H4">
         <v>0.80100000000000005</v>
@@ -1100,22 +1100,22 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>-1E-3</v>
+        <v>-3.4000000000000002E-2</v>
       </c>
       <c r="C5">
-        <v>-0.77800000000000002</v>
+        <v>-0.57799999999999996</v>
       </c>
       <c r="D5">
-        <v>-3.5000000000000003E-2</v>
+        <v>-4.1000000000000002E-2</v>
       </c>
       <c r="E5">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="F5">
-        <v>0.66800000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G5">
-        <v>0.58199999999999996</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="H5">
         <v>0.79</v>
@@ -1132,19 +1132,19 @@
         <v>-0.39300000000000002</v>
       </c>
       <c r="C6">
-        <v>-29.032</v>
+        <v>-35.304000000000002</v>
       </c>
       <c r="D6">
-        <v>-4.3999999999999997E-2</v>
+        <v>-3.4000000000000002E-2</v>
       </c>
       <c r="E6">
-        <v>-1.0999999999999999E-2</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="F6">
-        <v>0.68500000000000005</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="G6">
-        <v>0.65100000000000002</v>
+        <v>0.626</v>
       </c>
       <c r="H6">
         <v>0.82899999999999996</v>
@@ -1158,22 +1158,22 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.60799999999999998</v>
+        <v>0.629</v>
       </c>
       <c r="C7">
-        <v>-1.2869999999999999</v>
+        <v>-1.28</v>
       </c>
       <c r="D7">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E7">
-        <v>7.6999999999999999E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="F7">
-        <v>0.68400000000000005</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="G7">
-        <v>0.63900000000000001</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="H7">
         <v>0.77300000000000002</v>
@@ -1187,22 +1187,22 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.16700000000000001</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="C8">
-        <v>-2.181</v>
+        <v>-17.547000000000001</v>
       </c>
       <c r="D8">
-        <v>8.9999999999999993E-3</v>
+        <v>0.02</v>
       </c>
       <c r="E8">
-        <v>3.9E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="F8">
-        <v>0.69199999999999995</v>
+        <v>0.69299999999999995</v>
       </c>
       <c r="G8">
-        <v>0.60499999999999998</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="H8">
         <v>0.81899999999999995</v>
@@ -1216,19 +1216,19 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>-0.14299999999999999</v>
+        <v>-0.16700000000000001</v>
       </c>
       <c r="C9">
-        <v>-14.34</v>
+        <v>-14.43</v>
       </c>
       <c r="D9">
-        <v>6.8000000000000005E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="E9">
         <v>-1.2999999999999999E-2</v>
       </c>
       <c r="F9">
-        <v>0.66100000000000003</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="G9">
         <v>0.60799999999999998</v>
@@ -1245,22 +1245,22 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>0.248</v>
+        <v>0.252</v>
       </c>
       <c r="C10">
-        <v>0.27200000000000002</v>
+        <v>0.309</v>
       </c>
       <c r="D10">
-        <v>0.223</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="E10">
-        <v>0.253</v>
+        <v>0.254</v>
       </c>
       <c r="F10">
-        <v>0.91300000000000003</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="G10">
-        <v>0.60399999999999998</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="H10">
         <v>0.83899999999999997</v>
@@ -1274,22 +1274,22 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>0.66900000000000004</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="C11">
-        <v>0.78500000000000003</v>
+        <v>0.79600000000000004</v>
       </c>
       <c r="D11">
-        <v>0.13600000000000001</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="E11">
-        <v>0.20200000000000001</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="F11">
-        <v>0.877</v>
+        <v>0.876</v>
       </c>
       <c r="G11">
-        <v>0.70499999999999996</v>
+        <v>0.73199999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1300,19 +1300,19 @@
         <v>0.218</v>
       </c>
       <c r="C12">
-        <v>0.22900000000000001</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="D12">
-        <v>0.11700000000000001</v>
+        <v>0.109</v>
       </c>
       <c r="E12">
-        <v>0.104</v>
+        <v>0.105</v>
       </c>
       <c r="F12">
-        <v>0.90400000000000003</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="G12">
-        <v>0.79800000000000004</v>
+        <v>0.73499999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1320,22 +1320,22 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>0.376</v>
+        <v>0.38300000000000001</v>
       </c>
       <c r="C13">
-        <v>0.40699999999999997</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="D13">
-        <v>0.157</v>
+        <v>0.16</v>
       </c>
       <c r="E13">
-        <v>0.151</v>
+        <v>0.152</v>
       </c>
       <c r="F13">
-        <v>0.87</v>
+        <v>0.872</v>
       </c>
       <c r="G13">
-        <v>0.751</v>
+        <v>0.71099999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1343,22 +1343,22 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <v>0.60699999999999998</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="C14">
-        <v>0.63</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="D14">
-        <v>0.216</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="E14">
-        <v>0.20499999999999999</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="F14">
-        <v>0.875</v>
+        <v>0.876</v>
       </c>
       <c r="G14">
-        <v>0.74</v>
+        <v>0.74399999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1366,22 +1366,22 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="C15">
-        <v>0.73499999999999999</v>
+        <v>0.73899999999999999</v>
       </c>
       <c r="D15">
-        <v>0.193</v>
+        <v>0.18</v>
       </c>
       <c r="E15">
-        <v>0.17299999999999999</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="F15">
-        <v>0.85599999999999998</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="G15">
-        <v>0.72499999999999998</v>
+        <v>0.72799999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1389,22 +1389,22 @@
         <v>22</v>
       </c>
       <c r="B16">
-        <v>0.68799999999999994</v>
+        <v>0.621</v>
       </c>
       <c r="C16">
-        <v>0.76300000000000001</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="D16">
-        <v>0.16800000000000001</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="E16">
-        <v>0.191</v>
+        <v>0.183</v>
       </c>
       <c r="F16">
-        <v>0.90900000000000003</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="G16">
-        <v>0.57699999999999996</v>
+        <v>0.64900000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1412,22 +1412,22 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>0.59799999999999998</v>
+        <v>0.59899999999999998</v>
       </c>
       <c r="C17">
-        <v>0.64600000000000002</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="D17">
         <v>0.19500000000000001</v>
       </c>
       <c r="E17">
-        <v>0.14799999999999999</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="F17">
-        <v>0.79</v>
+        <v>0.79100000000000004</v>
       </c>
       <c r="G17">
-        <v>0.67100000000000004</v>
+        <v>0.72199999999999998</v>
       </c>
       <c r="H17">
         <v>0.76</v>
@@ -1444,19 +1444,19 @@
         <v>0.46</v>
       </c>
       <c r="C18">
-        <v>0.52800000000000002</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="D18">
-        <v>0.17699999999999999</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="E18">
         <v>0.154</v>
       </c>
       <c r="F18">
-        <v>0.86099999999999999</v>
+        <v>0.86</v>
       </c>
       <c r="G18">
-        <v>0.70699999999999996</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="H18">
         <v>0.84799999999999998</v>
@@ -1470,22 +1470,22 @@
         <v>25</v>
       </c>
       <c r="B19">
-        <v>0.69099999999999995</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="C19">
         <v>0.67300000000000004</v>
       </c>
       <c r="D19">
-        <v>0.17299999999999999</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="E19">
         <v>0.13800000000000001</v>
       </c>
       <c r="F19">
-        <v>0.72799999999999998</v>
+        <v>0.73</v>
       </c>
       <c r="G19">
-        <v>0.68300000000000005</v>
+        <v>0.68500000000000005</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1493,22 +1493,22 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <v>0.17599999999999999</v>
+        <v>0.183</v>
       </c>
       <c r="C20">
-        <v>0.42199999999999999</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="D20">
-        <v>0.115</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="E20">
-        <v>0.13400000000000001</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="F20">
-        <v>0.68600000000000005</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="G20">
-        <v>0.66100000000000003</v>
+        <v>0.66200000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1516,16 +1516,16 @@
         <v>27</v>
       </c>
       <c r="B21">
-        <v>0.44600000000000001</v>
+        <v>0.44800000000000001</v>
       </c>
       <c r="C21">
-        <v>0.45800000000000002</v>
+        <v>0.45</v>
       </c>
       <c r="D21">
-        <v>0.219</v>
+        <v>0.216</v>
       </c>
       <c r="E21">
-        <v>0.182</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="F21">
         <v>0.88300000000000001</v>
@@ -1548,16 +1548,16 @@
         <v>0.39400000000000002</v>
       </c>
       <c r="C22">
-        <v>0.34300000000000003</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="D22">
-        <v>0.11</v>
+        <v>0.112</v>
       </c>
       <c r="E22">
-        <v>3.2000000000000001E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="F22">
-        <v>0.66700000000000004</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="G22">
         <v>0.61599999999999999</v>
@@ -1574,13 +1574,13 @@
         <v>30</v>
       </c>
       <c r="B23">
-        <v>0.59099999999999997</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="C23">
-        <v>0.56000000000000005</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="D23">
-        <v>0.18099999999999999</v>
+        <v>0.182</v>
       </c>
       <c r="E23">
         <v>0.13800000000000001</v>
@@ -1589,7 +1589,7 @@
         <v>0.75800000000000001</v>
       </c>
       <c r="G23">
-        <v>0.67800000000000005</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="H23">
         <v>0.78600000000000003</v>
@@ -1608,7 +1608,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B2">
         <f>IF(accuracy_all!B2&gt;0,accuracy_all!B2,"&lt;0")</f>
-        <v>0.80800000000000005</v>
+        <v>0.80900000000000005</v>
       </c>
       <c r="C2">
         <f>IF(accuracy_all!C2&gt;0,accuracy_all!C2,"&lt;0")</f>
@@ -1656,15 +1656,15 @@
       </c>
       <c r="D2" s="1">
         <f>IF(accuracy_all!D2&gt;0,accuracy_all!D2,"&lt;0")</f>
-        <v>0.17899999999999999</v>
+        <v>0.18</v>
       </c>
       <c r="E2" s="1">
         <f>IF(accuracy_all!E2&gt;0,accuracy_all!E2,"&lt;0")</f>
-        <v>0.16800000000000001</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="F2">
         <f>IF(accuracy_all!F2&gt;0,accuracy_all!F2,"&lt;0")</f>
-        <v>0.67500000000000004</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="G2">
         <f>IF(accuracy_all!G2&gt;0,accuracy_all!G2,"&lt;0")</f>
@@ -1685,11 +1685,11 @@
       </c>
       <c r="B3">
         <f>IF(accuracy_all!B3&gt;0,accuracy_all!B3,"&lt;0")</f>
-        <v>0.34</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="C3">
         <f>IF(accuracy_all!C3&gt;0,accuracy_all!C3,"&lt;0")</f>
-        <v>0.19800000000000001</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>IF(accuracy_all!D3&gt;0,accuracy_all!D3,"&lt;0")</f>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="F3">
         <f>IF(accuracy_all!F3&gt;0,accuracy_all!F3,"&lt;0")</f>
-        <v>0.68899999999999995</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="G3">
         <f>IF(accuracy_all!G3&gt;0,accuracy_all!G3,"&lt;0")</f>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="B4">
         <f>IF(accuracy_all!B4&gt;0,accuracy_all!B4,"&lt;0")</f>
-        <v>0.45200000000000001</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="C4">
         <f>IF(accuracy_all!C4&gt;0,accuracy_all!C4,"&lt;0")</f>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="D4" s="1">
         <f>IF(accuracy_all!D4&gt;0,accuracy_all!D4,"&lt;0")</f>
-        <v>0.108</v>
+        <v>0.113</v>
       </c>
       <c r="E4" s="1">
         <f>IF(accuracy_all!E4&gt;0,accuracy_all!E4,"&lt;0")</f>
@@ -1738,11 +1738,11 @@
       </c>
       <c r="F4">
         <f>IF(accuracy_all!F4&gt;0,accuracy_all!F4,"&lt;0")</f>
-        <v>0.65200000000000002</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="G4">
         <f>IF(accuracy_all!G4&gt;0,accuracy_all!G4,"&lt;0")</f>
-        <v>0.6</v>
+        <v>0.60099999999999998</v>
       </c>
       <c r="H4">
         <f>IF(accuracy_all!H4&gt;0,accuracy_all!H4,"&lt;0")</f>
@@ -1775,11 +1775,11 @@
       </c>
       <c r="F5">
         <f>IF(accuracy_all!F5&gt;0,accuracy_all!F5,"&lt;0")</f>
-        <v>0.66800000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G5">
         <f>IF(accuracy_all!G5&gt;0,accuracy_all!G5,"&lt;0")</f>
-        <v>0.58199999999999996</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="H5">
         <f>IF(accuracy_all!H5&gt;0,accuracy_all!H5,"&lt;0")</f>
@@ -1812,11 +1812,11 @@
       </c>
       <c r="F6">
         <f>IF(accuracy_all!F6&gt;0,accuracy_all!F6,"&lt;0")</f>
-        <v>0.68500000000000005</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="G6">
         <f>IF(accuracy_all!G6&gt;0,accuracy_all!G6,"&lt;0")</f>
-        <v>0.65100000000000002</v>
+        <v>0.626</v>
       </c>
       <c r="H6">
         <f>IF(accuracy_all!H6&gt;0,accuracy_all!H6,"&lt;0")</f>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="B7">
         <f>IF(accuracy_all!B7&gt;0,accuracy_all!B7,"&lt;0")</f>
-        <v>0.60799999999999998</v>
+        <v>0.629</v>
       </c>
       <c r="C7" t="str">
         <f>IF(accuracy_all!C7&gt;0,accuracy_all!C7,"&lt;0")</f>
@@ -1841,19 +1841,19 @@
       </c>
       <c r="D7" s="1">
         <f>IF(accuracy_all!D7&gt;0,accuracy_all!D7,"&lt;0")</f>
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E7" s="1">
         <f>IF(accuracy_all!E7&gt;0,accuracy_all!E7,"&lt;0")</f>
-        <v>7.6999999999999999E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="F7">
         <f>IF(accuracy_all!F7&gt;0,accuracy_all!F7,"&lt;0")</f>
-        <v>0.68400000000000005</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="G7">
         <f>IF(accuracy_all!G7&gt;0,accuracy_all!G7,"&lt;0")</f>
-        <v>0.63900000000000001</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="H7">
         <f>IF(accuracy_all!H7&gt;0,accuracy_all!H7,"&lt;0")</f>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="B8">
         <f>IF(accuracy_all!B8&gt;0,accuracy_all!B8,"&lt;0")</f>
-        <v>0.16700000000000001</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="C8" t="str">
         <f>IF(accuracy_all!C8&gt;0,accuracy_all!C8,"&lt;0")</f>
@@ -1878,19 +1878,19 @@
       </c>
       <c r="D8" s="1">
         <f>IF(accuracy_all!D8&gt;0,accuracy_all!D8,"&lt;0")</f>
-        <v>8.9999999999999993E-3</v>
+        <v>0.02</v>
       </c>
       <c r="E8" s="1">
         <f>IF(accuracy_all!E8&gt;0,accuracy_all!E8,"&lt;0")</f>
-        <v>3.9E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="F8">
         <f>IF(accuracy_all!F8&gt;0,accuracy_all!F8,"&lt;0")</f>
-        <v>0.69199999999999995</v>
+        <v>0.69299999999999995</v>
       </c>
       <c r="G8">
         <f>IF(accuracy_all!G8&gt;0,accuracy_all!G8,"&lt;0")</f>
-        <v>0.60499999999999998</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="H8">
         <f>IF(accuracy_all!H8&gt;0,accuracy_all!H8,"&lt;0")</f>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="D9" s="1">
         <f>IF(accuracy_all!D9&gt;0,accuracy_all!D9,"&lt;0")</f>
-        <v>6.8000000000000005E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="E9" s="1" t="str">
         <f>IF(accuracy_all!E9&gt;0,accuracy_all!E9,"&lt;0")</f>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="F9">
         <f>IF(accuracy_all!F9&gt;0,accuracy_all!F9,"&lt;0")</f>
-        <v>0.66100000000000003</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="G9">
         <f>IF(accuracy_all!G9&gt;0,accuracy_all!G9,"&lt;0")</f>
@@ -1944,27 +1944,27 @@
       </c>
       <c r="B10">
         <f>IF(accuracy_all!B10&gt;0,accuracy_all!B10,"&lt;0")</f>
-        <v>0.248</v>
+        <v>0.252</v>
       </c>
       <c r="C10">
         <f>IF(accuracy_all!C10&gt;0,accuracy_all!C10,"&lt;0")</f>
-        <v>0.27200000000000002</v>
+        <v>0.309</v>
       </c>
       <c r="D10" s="1">
         <f>IF(accuracy_all!D10&gt;0,accuracy_all!D10,"&lt;0")</f>
-        <v>0.223</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="E10" s="1">
         <f>IF(accuracy_all!E10&gt;0,accuracy_all!E10,"&lt;0")</f>
-        <v>0.253</v>
+        <v>0.254</v>
       </c>
       <c r="F10">
         <f>IF(accuracy_all!F10&gt;0,accuracy_all!F10,"&lt;0")</f>
-        <v>0.91300000000000003</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="G10">
         <f>IF(accuracy_all!G10&gt;0,accuracy_all!G10,"&lt;0")</f>
-        <v>0.60399999999999998</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="H10">
         <f>IF(accuracy_all!H10&gt;0,accuracy_all!H10,"&lt;0")</f>
@@ -1981,27 +1981,27 @@
       </c>
       <c r="B11">
         <f>IF(accuracy_all!B11&gt;0,accuracy_all!B11,"&lt;0")</f>
-        <v>0.66900000000000004</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="C11">
         <f>IF(accuracy_all!C11&gt;0,accuracy_all!C11,"&lt;0")</f>
-        <v>0.78500000000000003</v>
+        <v>0.79600000000000004</v>
       </c>
       <c r="D11" s="1">
         <f>IF(accuracy_all!D11&gt;0,accuracy_all!D11,"&lt;0")</f>
-        <v>0.13600000000000001</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="E11" s="1">
         <f>IF(accuracy_all!E11&gt;0,accuracy_all!E11,"&lt;0")</f>
-        <v>0.20200000000000001</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="F11">
         <f>IF(accuracy_all!F11&gt;0,accuracy_all!F11,"&lt;0")</f>
-        <v>0.877</v>
+        <v>0.876</v>
       </c>
       <c r="G11">
         <f>IF(accuracy_all!G11&gt;0,accuracy_all!G11,"&lt;0")</f>
-        <v>0.70499999999999996</v>
+        <v>0.73199999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -2014,23 +2014,23 @@
       </c>
       <c r="C12">
         <f>IF(accuracy_all!C12&gt;0,accuracy_all!C12,"&lt;0")</f>
-        <v>0.22900000000000001</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="D12" s="1">
         <f>IF(accuracy_all!D12&gt;0,accuracy_all!D12,"&lt;0")</f>
-        <v>0.11700000000000001</v>
+        <v>0.109</v>
       </c>
       <c r="E12" s="1">
         <f>IF(accuracy_all!E12&gt;0,accuracy_all!E12,"&lt;0")</f>
-        <v>0.104</v>
+        <v>0.105</v>
       </c>
       <c r="F12">
         <f>IF(accuracy_all!F12&gt;0,accuracy_all!F12,"&lt;0")</f>
-        <v>0.90400000000000003</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="G12">
         <f>IF(accuracy_all!G12&gt;0,accuracy_all!G12,"&lt;0")</f>
-        <v>0.79800000000000004</v>
+        <v>0.73499999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2039,27 +2039,27 @@
       </c>
       <c r="B13">
         <f>IF(accuracy_all!B13&gt;0,accuracy_all!B13,"&lt;0")</f>
-        <v>0.376</v>
+        <v>0.38300000000000001</v>
       </c>
       <c r="C13">
         <f>IF(accuracy_all!C13&gt;0,accuracy_all!C13,"&lt;0")</f>
-        <v>0.40699999999999997</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="D13" s="1">
         <f>IF(accuracy_all!D13&gt;0,accuracy_all!D13,"&lt;0")</f>
-        <v>0.157</v>
+        <v>0.16</v>
       </c>
       <c r="E13" s="1">
         <f>IF(accuracy_all!E13&gt;0,accuracy_all!E13,"&lt;0")</f>
-        <v>0.151</v>
+        <v>0.152</v>
       </c>
       <c r="F13">
         <f>IF(accuracy_all!F13&gt;0,accuracy_all!F13,"&lt;0")</f>
-        <v>0.87</v>
+        <v>0.872</v>
       </c>
       <c r="G13">
         <f>IF(accuracy_all!G13&gt;0,accuracy_all!G13,"&lt;0")</f>
-        <v>0.751</v>
+        <v>0.71099999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2068,27 +2068,27 @@
       </c>
       <c r="B14">
         <f>IF(accuracy_all!B14&gt;0,accuracy_all!B14,"&lt;0")</f>
-        <v>0.60699999999999998</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="C14">
         <f>IF(accuracy_all!C14&gt;0,accuracy_all!C14,"&lt;0")</f>
-        <v>0.63</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="D14" s="1">
         <f>IF(accuracy_all!D14&gt;0,accuracy_all!D14,"&lt;0")</f>
-        <v>0.216</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="E14" s="1">
         <f>IF(accuracy_all!E14&gt;0,accuracy_all!E14,"&lt;0")</f>
-        <v>0.20499999999999999</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="F14">
         <f>IF(accuracy_all!F14&gt;0,accuracy_all!F14,"&lt;0")</f>
-        <v>0.875</v>
+        <v>0.876</v>
       </c>
       <c r="G14">
         <f>IF(accuracy_all!G14&gt;0,accuracy_all!G14,"&lt;0")</f>
-        <v>0.74</v>
+        <v>0.74399999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2097,27 +2097,27 @@
       </c>
       <c r="B15">
         <f>IF(accuracy_all!B15&gt;0,accuracy_all!B15,"&lt;0")</f>
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="C15">
         <f>IF(accuracy_all!C15&gt;0,accuracy_all!C15,"&lt;0")</f>
-        <v>0.73499999999999999</v>
+        <v>0.73899999999999999</v>
       </c>
       <c r="D15" s="1">
         <f>IF(accuracy_all!D15&gt;0,accuracy_all!D15,"&lt;0")</f>
-        <v>0.193</v>
+        <v>0.18</v>
       </c>
       <c r="E15" s="1">
         <f>IF(accuracy_all!E15&gt;0,accuracy_all!E15,"&lt;0")</f>
-        <v>0.17299999999999999</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="F15">
         <f>IF(accuracy_all!F15&gt;0,accuracy_all!F15,"&lt;0")</f>
-        <v>0.85599999999999998</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="G15">
         <f>IF(accuracy_all!G15&gt;0,accuracy_all!G15,"&lt;0")</f>
-        <v>0.72499999999999998</v>
+        <v>0.72799999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -2126,27 +2126,27 @@
       </c>
       <c r="B16">
         <f>IF(accuracy_all!B16&gt;0,accuracy_all!B16,"&lt;0")</f>
-        <v>0.68799999999999994</v>
+        <v>0.621</v>
       </c>
       <c r="C16">
         <f>IF(accuracy_all!C16&gt;0,accuracy_all!C16,"&lt;0")</f>
-        <v>0.76300000000000001</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="D16" s="1">
         <f>IF(accuracy_all!D16&gt;0,accuracy_all!D16,"&lt;0")</f>
-        <v>0.16800000000000001</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="E16" s="1">
         <f>IF(accuracy_all!E16&gt;0,accuracy_all!E16,"&lt;0")</f>
-        <v>0.191</v>
+        <v>0.183</v>
       </c>
       <c r="F16">
         <f>IF(accuracy_all!F16&gt;0,accuracy_all!F16,"&lt;0")</f>
-        <v>0.90900000000000003</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="G16">
         <f>IF(accuracy_all!G16&gt;0,accuracy_all!G16,"&lt;0")</f>
-        <v>0.57699999999999996</v>
+        <v>0.64900000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -2155,11 +2155,11 @@
       </c>
       <c r="B17">
         <f>IF(accuracy_all!B17&gt;0,accuracy_all!B17,"&lt;0")</f>
-        <v>0.59799999999999998</v>
+        <v>0.59899999999999998</v>
       </c>
       <c r="C17">
         <f>IF(accuracy_all!C17&gt;0,accuracy_all!C17,"&lt;0")</f>
-        <v>0.64600000000000002</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="D17" s="1">
         <f>IF(accuracy_all!D17&gt;0,accuracy_all!D17,"&lt;0")</f>
@@ -2167,15 +2167,15 @@
       </c>
       <c r="E17" s="1">
         <f>IF(accuracy_all!E17&gt;0,accuracy_all!E17,"&lt;0")</f>
-        <v>0.14799999999999999</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="F17">
         <f>IF(accuracy_all!F17&gt;0,accuracy_all!F17,"&lt;0")</f>
-        <v>0.79</v>
+        <v>0.79100000000000004</v>
       </c>
       <c r="G17">
         <f>IF(accuracy_all!G17&gt;0,accuracy_all!G17,"&lt;0")</f>
-        <v>0.67100000000000004</v>
+        <v>0.72199999999999998</v>
       </c>
       <c r="H17">
         <f>IF(accuracy_all!H17&gt;0,accuracy_all!H17,"&lt;0")</f>
@@ -2196,11 +2196,11 @@
       </c>
       <c r="C18">
         <f>IF(accuracy_all!C18&gt;0,accuracy_all!C18,"&lt;0")</f>
-        <v>0.52800000000000002</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="D18" s="1">
         <f>IF(accuracy_all!D18&gt;0,accuracy_all!D18,"&lt;0")</f>
-        <v>0.17699999999999999</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="E18" s="1">
         <f>IF(accuracy_all!E18&gt;0,accuracy_all!E18,"&lt;0")</f>
@@ -2208,11 +2208,11 @@
       </c>
       <c r="F18">
         <f>IF(accuracy_all!F18&gt;0,accuracy_all!F18,"&lt;0")</f>
-        <v>0.86099999999999999</v>
+        <v>0.86</v>
       </c>
       <c r="G18">
         <f>IF(accuracy_all!G18&gt;0,accuracy_all!G18,"&lt;0")</f>
-        <v>0.70699999999999996</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="H18">
         <f>IF(accuracy_all!H18&gt;0,accuracy_all!H18,"&lt;0")</f>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="B19">
         <f>IF(accuracy_all!B19&gt;0,accuracy_all!B19,"&lt;0")</f>
-        <v>0.69099999999999995</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="C19">
         <f>IF(accuracy_all!C19&gt;0,accuracy_all!C19,"&lt;0")</f>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="D19" s="1">
         <f>IF(accuracy_all!D19&gt;0,accuracy_all!D19,"&lt;0")</f>
-        <v>0.17299999999999999</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="E19" s="1">
         <f>IF(accuracy_all!E19&gt;0,accuracy_all!E19,"&lt;0")</f>
@@ -2245,11 +2245,11 @@
       </c>
       <c r="F19">
         <f>IF(accuracy_all!F19&gt;0,accuracy_all!F19,"&lt;0")</f>
-        <v>0.72799999999999998</v>
+        <v>0.73</v>
       </c>
       <c r="G19">
         <f>IF(accuracy_all!G19&gt;0,accuracy_all!G19,"&lt;0")</f>
-        <v>0.68300000000000005</v>
+        <v>0.68500000000000005</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -2258,27 +2258,27 @@
       </c>
       <c r="B20">
         <f>IF(accuracy_all!B20&gt;0,accuracy_all!B20,"&lt;0")</f>
-        <v>0.17599999999999999</v>
+        <v>0.183</v>
       </c>
       <c r="C20">
         <f>IF(accuracy_all!C20&gt;0,accuracy_all!C20,"&lt;0")</f>
-        <v>0.42199999999999999</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="D20" s="1">
         <f>IF(accuracy_all!D20&gt;0,accuracy_all!D20,"&lt;0")</f>
-        <v>0.115</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="E20" s="1">
         <f>IF(accuracy_all!E20&gt;0,accuracy_all!E20,"&lt;0")</f>
-        <v>0.13400000000000001</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="F20">
         <f>IF(accuracy_all!F20&gt;0,accuracy_all!F20,"&lt;0")</f>
-        <v>0.68600000000000005</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="G20">
         <f>IF(accuracy_all!G20&gt;0,accuracy_all!G20,"&lt;0")</f>
-        <v>0.66100000000000003</v>
+        <v>0.66200000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -2287,19 +2287,19 @@
       </c>
       <c r="B21">
         <f>IF(accuracy_all!B21&gt;0,accuracy_all!B21,"&lt;0")</f>
-        <v>0.44600000000000001</v>
+        <v>0.44800000000000001</v>
       </c>
       <c r="C21">
         <f>IF(accuracy_all!C21&gt;0,accuracy_all!C21,"&lt;0")</f>
-        <v>0.45800000000000002</v>
+        <v>0.45</v>
       </c>
       <c r="D21" s="1">
         <f>IF(accuracy_all!D21&gt;0,accuracy_all!D21,"&lt;0")</f>
-        <v>0.219</v>
+        <v>0.216</v>
       </c>
       <c r="E21" s="1">
         <f>IF(accuracy_all!E21&gt;0,accuracy_all!E21,"&lt;0")</f>
-        <v>0.182</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="F21">
         <f>IF(accuracy_all!F21&gt;0,accuracy_all!F21,"&lt;0")</f>
@@ -2328,19 +2328,19 @@
       </c>
       <c r="C22">
         <f>IF(accuracy_all!C22&gt;0,accuracy_all!C22,"&lt;0")</f>
-        <v>0.34300000000000003</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="D22" s="1">
         <f>IF(accuracy_all!D22&gt;0,accuracy_all!D22,"&lt;0")</f>
-        <v>0.11</v>
+        <v>0.112</v>
       </c>
       <c r="E22" s="1">
         <f>IF(accuracy_all!E22&gt;0,accuracy_all!E22,"&lt;0")</f>
-        <v>3.2000000000000001E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="F22">
         <f>IF(accuracy_all!F22&gt;0,accuracy_all!F22,"&lt;0")</f>
-        <v>0.66700000000000004</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="G22">
         <f>IF(accuracy_all!G22&gt;0,accuracy_all!G22,"&lt;0")</f>
@@ -2367,7 +2367,7 @@
       </c>
       <c r="D23" s="1">
         <f>IF(accuracy_all!D23&gt;0,accuracy_all!D23,"&lt;0")</f>
-        <v>0.18099999999999999</v>
+        <v>0.182</v>
       </c>
       <c r="E23" s="1">
         <f>IF(accuracy_all!E23&gt;0,accuracy_all!E23,"&lt;0")</f>

</xml_diff>